<commit_message>
Change to dot from comma and save as csv + description. Deleted unnecessary data columns
</commit_message>
<xml_diff>
--- a/data/kongepanel_upd_oppdatert_februar.xlsx
+++ b/data/kongepanel_upd_oppdatert_februar.xlsx
@@ -1715,7 +1715,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
-    <numFmt numFmtId="173" formatCode="d/m/yyyy;@"/>
+    <numFmt numFmtId="167" formatCode="d/m/yyyy;@"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -1994,15 +1994,15 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="17"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="18" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="18" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="173" fontId="1" fillId="9" borderId="0" xfId="17" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="1" fillId="9" borderId="0" xfId="17" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="173" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="16" fillId="8" borderId="0" xfId="16" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="18" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="1" fillId="9" borderId="0" xfId="17" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="16" fillId="8" borderId="0" xfId="16" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="16" fillId="8" borderId="0" xfId="16" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="8" borderId="0" xfId="16"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="19" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>

</xml_diff>